<commit_message>
major addition of new data
</commit_message>
<xml_diff>
--- a/NH_HealthCost_data/45380 Colonoscopy with biopsy (outpatient).xlsx
+++ b/NH_HealthCost_data/45380 Colonoscopy with biopsy (outpatient).xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teresarokos/Desktop/Thesis Research/NH HealthCost data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teresarokos/Desktop/Thesis Research/Thesis_Hospital_Costs/NH_HealthCost_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E20A1C-9FA1-5847-9954-AFF83FAC6B37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFBE4ED-CBEA-8345-AF5B-56A630B74138}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27640" windowHeight="16060" activeTab="4" xr2:uid="{10692E2F-075C-8245-B24A-BFB9617158D9}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27640" windowHeight="16060" xr2:uid="{10692E2F-075C-8245-B24A-BFB9617158D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Anthem - NH" sheetId="1" r:id="rId1"/>
+    <sheet name="Anthem NH" sheetId="1" r:id="rId1"/>
     <sheet name="CIGNA" sheetId="2" r:id="rId2"/>
     <sheet name="Harvard Pilgrim HC" sheetId="3" r:id="rId3"/>
     <sheet name="Other" sheetId="4" r:id="rId4"/>
@@ -10798,8 +10798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545EEBE9-A5A8-7541-9DD6-8703FA470963}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12221,7 +12221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A577D5-E9A8-BB43-9129-BA3CD01E076F}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>

</xml_diff>